<commit_message>
new build is getting there
</commit_message>
<xml_diff>
--- a/Functional skills maths/assets/bios/bios.xlsx
+++ b/Functional skills maths/assets/bios/bios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\GitHub\Functional skills site newbuild\backgroundfiles\assets\bios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984A1D36-0DA5-4B25-88A5-6F57380FC3E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94512511-E61F-4A63-9F7E-692509817ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{E76E8D28-8132-4DAF-A3A8-FE7EE221AAEA}"/>
+    <workbookView xWindow="29160" yWindow="1965" windowWidth="19095" windowHeight="10590" xr2:uid="{E76E8D28-8132-4DAF-A3A8-FE7EE221AAEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -71,6 +71,21 @@
   </si>
   <si>
     <t>I'm a data coach and ex maths teacher joining the team to help build out their online platform</t>
+  </si>
+  <si>
+    <t>calendly link</t>
+  </si>
+  <si>
+    <t>https://calendly.com/nick-griffiths-22/strategy-meeting-clone</t>
+  </si>
+  <si>
+    <t>Yoda 2</t>
+  </si>
+  <si>
+    <t>Yoda 3</t>
+  </si>
+  <si>
+    <t>Yoda 4</t>
   </si>
 </sst>
 </file>
@@ -438,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCC286A0-CCB5-4479-A456-9CDA98674DC7}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -449,9 +464,10 @@
     <col min="1" max="2" width="43" style="1" customWidth="1"/>
     <col min="3" max="3" width="78.6328125" style="1" customWidth="1"/>
     <col min="4" max="4" width="43" style="1" customWidth="1"/>
+    <col min="5" max="5" width="53.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,8 +480,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -478,8 +497,11 @@
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -491,12 +513,69 @@
       </c>
       <c r="D3" s="2" t="s">
         <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{8FE427AA-AF17-4A07-B905-C8F915379F45}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{C0B0798F-FB14-4EFF-BA62-CB162F4A9DB9}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{A6BFBCCA-A341-44F8-816D-AD97451607C9}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{C8E020A7-33A2-455E-B321-787C0D11CB83}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{C8F5CD26-DB5F-4DAD-B07D-B6BD1F1E66CE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>